<commit_message>
fix single numeric train
</commit_message>
<xml_diff>
--- a/result/feats_seletor_result.xlsx
+++ b/result/feats_seletor_result.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>fold</t>
   </si>
@@ -73,21 +73,21 @@
     <t>credit.history</t>
   </si>
   <si>
+    <t>installment.rate.in.percentage.of.disposable.income</t>
+  </si>
+  <si>
     <t>other.debtors.or.guarantors</t>
   </si>
   <si>
-    <t>installment.rate.in.percentage.of.disposable.income</t>
+    <t>present.residence.since</t>
+  </si>
+  <si>
+    <t>present.employment.since</t>
   </si>
   <si>
     <t>housing</t>
   </si>
   <si>
-    <t>present.employment.since</t>
-  </si>
-  <si>
-    <t>present.residence.since</t>
-  </si>
-  <si>
     <t>step</t>
   </si>
   <si>
@@ -121,19 +121,19 @@
     <t>['credit.history']</t>
   </si>
   <si>
+    <t>['installment.rate.in.percentage.of.disposable.income']</t>
+  </si>
+  <si>
     <t>['other.debtors.or.guarantors']</t>
   </si>
   <si>
-    <t>['installment.rate.in.percentage.of.disposable.income']</t>
+    <t>['present.residence.since']</t>
+  </si>
+  <si>
+    <t>['present.employment.since']</t>
   </si>
   <si>
     <t>['housing']</t>
-  </si>
-  <si>
-    <t>['present.employment.since']</t>
-  </si>
-  <si>
-    <t>['present.residence.since']</t>
   </si>
 </sst>
 </file>
@@ -522,16 +522,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.9046603830041892</v>
+        <v>0.9098967684021544</v>
       </c>
       <c r="D2">
-        <v>0.820952380952381</v>
+        <v>0.8230952380952381</v>
       </c>
       <c r="E2">
-        <v>0.6511594853381208</v>
+        <v>0.6674521244763615</v>
       </c>
       <c r="F2">
-        <v>0.5095238095238095</v>
+        <v>0.5428571428571428</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -542,16 +542,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.8607532914422501</v>
+        <v>0.8844703770197486</v>
       </c>
       <c r="D3">
-        <v>0.7713690476190476</v>
+        <v>0.7359523809523809</v>
       </c>
       <c r="E3">
-        <v>0.5589168162776781</v>
+        <v>0.6078994614003591</v>
       </c>
       <c r="F3">
-        <v>0.4642857142857143</v>
+        <v>0.4095238095238095</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -562,16 +562,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.8718264635603346</v>
+        <v>0.9179136798088411</v>
       </c>
       <c r="D4">
-        <v>0.7498800959232614</v>
+        <v>0.7521582733812949</v>
       </c>
       <c r="E4">
-        <v>0.5745967741935484</v>
+        <v>0.6682795698924732</v>
       </c>
       <c r="F4">
-        <v>0.4171462829736211</v>
+        <v>0.4383693045563549</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -582,16 +582,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.9111932497013142</v>
+        <v>0.8769489247311828</v>
       </c>
       <c r="D5">
-        <v>0.7923261390887291</v>
+        <v>0.8164268585131894</v>
       </c>
       <c r="E5">
-        <v>0.6515232974910394</v>
+        <v>0.5932795698924731</v>
       </c>
       <c r="F5">
-        <v>0.4910071942446043</v>
+        <v>0.5038369304556355</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -602,16 +602,16 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.9152703106332138</v>
+        <v>0.8710722819593787</v>
       </c>
       <c r="D6">
-        <v>0.7834532374100719</v>
+        <v>0.8317745803357314</v>
       </c>
       <c r="E6">
-        <v>0.662768817204301</v>
+        <v>0.5732078853046595</v>
       </c>
       <c r="F6">
-        <v>0.4520383693045564</v>
+        <v>0.5553956834532374</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -622,16 +622,16 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.8927407396682604</v>
+        <v>0.892060406384261</v>
       </c>
       <c r="D7">
-        <v>0.7820970827355334</v>
+        <v>0.7887374461979915</v>
       </c>
       <c r="E7">
-        <v>0.6197930381009376</v>
+        <v>0.6220237221932653</v>
       </c>
       <c r="F7">
-        <v>0.4668002740664611</v>
+        <v>0.489996574169236</v>
       </c>
     </row>
   </sheetData>
@@ -669,19 +669,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2">
-        <v>474.3924796283245</v>
+        <v>471.2633125782013</v>
       </c>
       <c r="E2">
-        <v>0.2741644213920543</v>
+        <v>0.2709371718059145</v>
       </c>
       <c r="F2">
-        <v>0.2741644213920543</v>
+        <v>0.2709371718059145</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -695,13 +695,13 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>331.2164318680764</v>
+        <v>310.8317297816276</v>
       </c>
       <c r="E3">
-        <v>0.1914190576330335</v>
+        <v>0.178702367714227</v>
       </c>
       <c r="F3">
-        <v>0.4655834790250879</v>
+        <v>0.4496395395201415</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -715,13 +715,13 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>173.6334265619517</v>
+        <v>167.268590426445</v>
       </c>
       <c r="E4">
-        <v>0.1003475180824408</v>
+        <v>0.09616551429426751</v>
       </c>
       <c r="F4">
-        <v>0.5659309971075287</v>
+        <v>0.545805053814409</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -729,19 +729,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5">
-        <v>114.7938145190477</v>
+        <v>127.706204354763</v>
       </c>
       <c r="E5">
-        <v>0.06634249295363917</v>
+        <v>0.07342043589316341</v>
       </c>
       <c r="F5">
-        <v>0.6322734900611678</v>
+        <v>0.6192254897075724</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -749,19 +749,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6">
-        <v>99.98604431152344</v>
+        <v>101.4248958945274</v>
       </c>
       <c r="E6">
-        <v>0.05778467653497855</v>
+        <v>0.05831087146172149</v>
       </c>
       <c r="F6">
-        <v>0.6900581665961464</v>
+        <v>0.6775363611692939</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -769,19 +769,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7">
-        <v>92.91162899136542</v>
+        <v>101.0704591661692</v>
       </c>
       <c r="E7">
-        <v>0.05369617794735801</v>
+        <v>0.05810709984996549</v>
       </c>
       <c r="F7">
-        <v>0.7437543445435044</v>
+        <v>0.7356434610192595</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -789,19 +789,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8">
-        <v>88.09924777746201</v>
+        <v>95.67135408818721</v>
       </c>
       <c r="E8">
-        <v>0.05091497089268141</v>
+        <v>0.05500306390855399</v>
       </c>
       <c r="F8">
-        <v>0.7946693154361858</v>
+        <v>0.7906465249278135</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -809,19 +809,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9">
-        <v>61.08298815488815</v>
+        <v>73.13659776449202</v>
       </c>
       <c r="E9">
-        <v>0.03530153369527134</v>
+        <v>0.04204745505312398</v>
       </c>
       <c r="F9">
-        <v>0.8299708491314571</v>
+        <v>0.8326939799809375</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -829,19 +829,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10">
-        <v>57.55395911931992</v>
+        <v>64.2222418129444</v>
       </c>
       <c r="E10">
-        <v>0.03326201105281637</v>
+        <v>0.03692244250595535</v>
       </c>
       <c r="F10">
-        <v>0.8632328601842735</v>
+        <v>0.8696164224868929</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -849,19 +849,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11">
-        <v>42.12057256698608</v>
+        <v>44.09301280975342</v>
       </c>
       <c r="E11">
-        <v>0.02434263379465319</v>
+        <v>0.02534981159836023</v>
       </c>
       <c r="F11">
-        <v>0.8875754939789267</v>
+        <v>0.8949662340852531</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -869,19 +869,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12">
-        <v>41.07773293256759</v>
+        <v>41.33051123321057</v>
       </c>
       <c r="E12">
-        <v>0.0237399481761985</v>
+        <v>0.02376160317160369</v>
       </c>
       <c r="F12">
-        <v>0.9113154421551252</v>
+        <v>0.9187278372568568</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -889,19 +889,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13">
-        <v>40.21781942844391</v>
+        <v>38.6174860715866</v>
       </c>
       <c r="E13">
-        <v>0.02324298058411105</v>
+        <v>0.02220183956448712</v>
       </c>
       <c r="F13">
-        <v>0.9345584227392362</v>
+        <v>0.9409296768213439</v>
       </c>
     </row>
   </sheetData>
@@ -911,7 +911,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -939,19 +939,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2">
-        <v>474.3924796283245</v>
+        <v>471.2633125782013</v>
       </c>
       <c r="E2">
-        <v>0.2741644213920543</v>
+        <v>0.2709371718059145</v>
       </c>
       <c r="F2">
-        <v>0.2741644213920543</v>
+        <v>0.2709371718059145</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -965,13 +965,13 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>331.2164318680764</v>
+        <v>310.8317297816276</v>
       </c>
       <c r="E3">
-        <v>0.1914190576330335</v>
+        <v>0.178702367714227</v>
       </c>
       <c r="F3">
-        <v>0.4655834790250879</v>
+        <v>0.4496395395201415</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -979,19 +979,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4">
-        <v>114.7938145190477</v>
+        <v>127.706204354763</v>
       </c>
       <c r="E4">
-        <v>0.06634249295363917</v>
+        <v>0.07342043589316341</v>
       </c>
       <c r="F4">
-        <v>0.6322734900611678</v>
+        <v>0.6192254897075724</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -999,19 +999,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5">
-        <v>99.98604431152344</v>
+        <v>101.4248958945274</v>
       </c>
       <c r="E5">
-        <v>0.05778467653497855</v>
+        <v>0.05831087146172149</v>
       </c>
       <c r="F5">
-        <v>0.6900581665961464</v>
+        <v>0.6775363611692939</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1019,19 +1019,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6">
-        <v>92.91162899136542</v>
+        <v>101.0704591661692</v>
       </c>
       <c r="E6">
-        <v>0.05369617794735801</v>
+        <v>0.05810709984996549</v>
       </c>
       <c r="F6">
-        <v>0.7437543445435044</v>
+        <v>0.7356434610192595</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1039,19 +1039,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7">
-        <v>88.09924777746201</v>
+        <v>95.67135408818721</v>
       </c>
       <c r="E7">
-        <v>0.05091497089268141</v>
+        <v>0.05500306390855399</v>
       </c>
       <c r="F7">
-        <v>0.7946693154361858</v>
+        <v>0.7906465249278135</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1059,39 +1059,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8">
-        <v>61.08298815488815</v>
+        <v>64.2222418129444</v>
       </c>
       <c r="E8">
-        <v>0.03530153369527134</v>
+        <v>0.03692244250595535</v>
       </c>
       <c r="F8">
-        <v>0.8299708491314571</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>42.12057256698608</v>
-      </c>
-      <c r="E9">
-        <v>0.02434263379465319</v>
-      </c>
-      <c r="F9">
-        <v>0.8875754939789267</v>
+        <v>0.8696164224868929</v>
       </c>
     </row>
   </sheetData>
@@ -1129,10 +1109,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.7076186193902021</v>
+        <v>0.7079597464885234</v>
       </c>
       <c r="D2">
-        <v>0.2076186193902021</v>
+        <v>0.2079597464885234</v>
       </c>
       <c r="E2" t="s">
         <v>27</v>
@@ -1146,10 +1126,10 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.7511323227132579</v>
+        <v>0.7553816375471051</v>
       </c>
       <c r="D3">
-        <v>0.04351370332305582</v>
+        <v>0.04742189105858163</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -1163,10 +1143,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.7443105515587529</v>
+        <v>0.7485474477560808</v>
       </c>
       <c r="D4">
-        <v>-0.006821771154504996</v>
+        <v>-0.006834189791024237</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
@@ -1180,10 +1160,10 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.7668985097636176</v>
+        <v>0.7674050188420692</v>
       </c>
       <c r="D5">
-        <v>0.0157661870503597</v>
+        <v>0.01202338129496416</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -1197,10 +1177,10 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.7706742034943473</v>
+        <v>0.7715508735868448</v>
       </c>
       <c r="D6">
-        <v>0.003775693730729723</v>
+        <v>0.004145854744775579</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -1214,10 +1194,10 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.7720161870503597</v>
+        <v>0.7766170777663584</v>
       </c>
       <c r="D7">
-        <v>0.001341983556012338</v>
+        <v>0.005066204179513534</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -1231,10 +1211,10 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0.7759345666324083</v>
+        <v>0.7838550017129153</v>
       </c>
       <c r="D8">
-        <v>0.003918379582048659</v>
+        <v>0.007237923946556979</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -1248,10 +1228,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0.7870386262418636</v>
+        <v>0.7826848235697156</v>
       </c>
       <c r="D9">
-        <v>0.01110405960945526</v>
+        <v>-0.001170178143199752</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
@@ -1265,10 +1245,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>0.7859118705035971</v>
+        <v>0.7951287255909558</v>
       </c>
       <c r="D10">
-        <v>-0.001126755738266483</v>
+        <v>0.01127372387804049</v>
       </c>
       <c r="E10" t="s">
         <v>35</v>
@@ -1282,10 +1262,10 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>0.7892762076053442</v>
+        <v>0.793486125385406</v>
       </c>
       <c r="D11">
-        <v>0.002237581363480623</v>
+        <v>-0.001642600205549849</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
@@ -1299,10 +1279,10 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0.7889172661870504</v>
+        <v>0.7958266529633435</v>
       </c>
       <c r="D12">
-        <v>-0.0003589414182938455</v>
+        <v>0.0006979273723877188</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
@@ -1316,10 +1296,10 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>0.7827522267899967</v>
+        <v>0.7943931997259335</v>
       </c>
       <c r="D13">
-        <v>-0.006523980815347552</v>
+        <v>-0.0007355258650223462</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>

</xml_diff>